<commit_message>
Creacion de formato Excel Vertical
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Tasas-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6578DFF4-0CE5-418F-986C-8A72FD965967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16422B7F-F157-4BFA-B614-FE99C4E15D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="630" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="420" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>URL</t>
   </si>
@@ -69,13 +69,19 @@
   </si>
   <si>
     <t>MXN</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>PEN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -105,6 +111,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -120,7 +134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -128,78 +142,32 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -217,6 +185,9 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
@@ -231,10 +202,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}" name="Tabla1" displayName="Tabla1" ref="A1:C7" totalsRowShown="0">
-  <autoFilter ref="A1:C7" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}" name="Tabla1" displayName="Tabla1" ref="A1:C9" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C9" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8451EFC4-375F-4EF1-B2A2-7878C751B650}" name="URL" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{8451EFC4-375F-4EF1-B2A2-7878C751B650}" name="URL" dataDxfId="3">
       <calculatedColumnFormula>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{30A2418A-0C4F-4155-8F56-B5A5880AB528}" name="TO" dataDxfId="2"/>
@@ -569,121 +540,139 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.25" customWidth="1"/>
+    <col min="1" max="1" width="67.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="str">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
         <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
         <v>https://www.oanda.com/currency-converter/es/?from=EUR&amp;to=USD&amp;amount=1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="str">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
         <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
         <v>https://www.oanda.com/currency-converter/es/?from=CNY&amp;to=GBP&amp;amount=1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="str">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
         <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
         <v>https://www.oanda.com/currency-converter/es/?from=BRL&amp;to=USD&amp;amount=1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="str">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
         <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
         <v>https://www.oanda.com/currency-converter/es/?from=KRW&amp;to=USD&amp;amount=1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="str">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
         <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
         <v>https://www.oanda.com/currency-converter/es/?from=CNY&amp;to=COP&amp;amount=1</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="str">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
         <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
         <v>https://www.oanda.com/currency-converter/es/?from=MXN&amp;to=HNL&amp;amount=1</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
+        <v>https://www.oanda.com/currency-converter/es/?from=JPY&amp;to=USD&amp;amount=1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
+        <v>https://www.oanda.com/currency-converter/es/?from=PEN&amp;to=USD&amp;amount=1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="1"/>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G19" s="1"/>

</xml_diff>

<commit_message>
Cambio de Nombre para el programa
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augusto.machado\Desktop\Tasas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87392CEA-9E1B-43E0-A40A-B2C5551ED4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E79075A-7321-4D3D-9E63-AB7B2DF0E06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>URL</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>COP</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>MXN</t>
+  </si>
+  <si>
+    <t>HNL</t>
   </si>
   <si>
     <t>JPY</t>
@@ -182,8 +191,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}" name="Tabla1" displayName="Tabla1" ref="A1:C6" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:C6" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}" name="Tabla1" displayName="Tabla1" ref="A1:C7" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:C7" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8451EFC4-375F-4EF1-B2A2-7878C751B650}" name="URL" dataDxfId="2">
       <calculatedColumnFormula>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</calculatedColumnFormula>
@@ -520,7 +529,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -580,10 +589,10 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
-        <v>https://www.oanda.com/currency-converter/es/?from=BRL&amp;to=USD&amp;amount=1</v>
+        <v>https://www.oanda.com/currency-converter/es/?from=GBP&amp;to=USD&amp;amount=1</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>4</v>
@@ -592,20 +601,27 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
-        <v>https://www.oanda.com/currency-converter/es/?from=JPY&amp;to=COP&amp;amount=1</v>
+        <v>https://www.oanda.com/currency-converter/es/?from=MXN&amp;to=HNL&amp;amount=1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="A7" s="3" t="str">
+        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
+        <v>https://www.oanda.com/currency-converter/es/?from=JPY&amp;to=USD&amp;amount=1</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Configuracion sobre el tiempo y busqueda de datos
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augusto.machado\Desktop\Tasas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E79075A-7321-4D3D-9E63-AB7B2DF0E06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95C4601-CEE7-428D-BE26-7476A3DAC871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
   <si>
     <t>URL</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>JPY</t>
+  </si>
+  <si>
+    <t>HKD</t>
   </si>
 </sst>
 </file>
@@ -135,7 +138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -145,7 +148,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -191,8 +193,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}" name="Tabla1" displayName="Tabla1" ref="A1:C7" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:C7" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}" name="Tabla1" displayName="Tabla1" ref="A1:C18" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:C18" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8451EFC4-375F-4EF1-B2A2-7878C751B650}" name="URL" dataDxfId="2">
       <calculatedColumnFormula>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</calculatedColumnFormula>
@@ -526,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -591,10 +593,10 @@
         <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
         <v>https://www.oanda.com/currency-converter/es/?from=GBP&amp;to=USD&amp;amount=1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -603,10 +605,10 @@
         <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
         <v>https://www.oanda.com/currency-converter/es/?from=MXN&amp;to=HNL&amp;amount=1</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="1"/>
@@ -616,47 +618,183 @@
         <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
         <v>https://www.oanda.com/currency-converter/es/?from=JPY&amp;to=USD&amp;amount=1</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="A8" s="3" t="str">
+        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
+        <v>https://www.oanda.com/currency-converter/es/?from=EUR&amp;to=COP&amp;amount=1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="A9" s="3" t="str">
+        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
+        <v>https://www.oanda.com/currency-converter/es/?from=EUR&amp;to=USD&amp;amount=1</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="3" t="str">
+        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
+        <v>https://www.oanda.com/currency-converter/es/?from=CNY&amp;to=USD&amp;amount=1</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="3" t="str">
+        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
+        <v>https://www.oanda.com/currency-converter/es/?from=JPY&amp;to=USD&amp;amount=1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="3" t="str">
+        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
+        <v>https://www.oanda.com/currency-converter/es/?from=CNY&amp;to=COP&amp;amount=1</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="str">
+        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
+        <v>https://www.oanda.com/currency-converter/es/?from=JPY&amp;to=COP&amp;amount=1</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="str">
+        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
+        <v>https://www.oanda.com/currency-converter/es/?from=BRL&amp;to=USD&amp;amount=1</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="str">
+        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
+        <v>https://www.oanda.com/currency-converter/es/?from=JPY&amp;to=HNL&amp;amount=1</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="str">
+        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
+        <v>https://www.oanda.com/currency-converter/es/?from=MXN&amp;to=HNL&amp;amount=1</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="str">
+        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
+        <v>https://www.oanda.com/currency-converter/es/?from=HKD&amp;to=USD&amp;amount=1</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="str">
+        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
+        <v>https://www.oanda.com/currency-converter/es/?from=HKD&amp;to=HNL&amp;amount=1</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
       <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Use UserAgent for create ExchangeRate Colombia
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Tasas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DC522B-35C1-495C-9787-56A8B371EFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1210C2-3EE8-441D-A9CF-4CF91D1E3F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -131,7 +131,7 @@
     <t>https://www.banrep.gov.co/es</t>
   </si>
   <si>
-    <t>#block-banrepindicatorsblock &gt; div &gt; div.column.large-3.indicator.indicator--trm &gt; div.indicator__value</t>
+    <t>#block-banrepindicatorsblock &gt; div &gt; div.column.large-3.indicator.indicator--trm &gt; div.indicator__value &gt; a</t>
   </si>
 </sst>
 </file>
@@ -198,7 +198,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -209,6 +209,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -629,7 +631,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -869,18 +871,19 @@
       <c r="H10" t="s">
         <v>14</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="E11" s="1"/>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -902,6 +905,7 @@
     </row>
     <row r="19" spans="6:9" x14ac:dyDescent="0.25">
       <c r="G19" s="1"/>
+      <c r="I19" s="1"/>
     </row>
     <row r="21" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F21" s="1"/>

</xml_diff>

<commit_message>
Creacion de la base de datos sobre un .txt
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Tasas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1210C2-3EE8-441D-A9CF-4CF91D1E3F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86588445-72D1-4A17-8DD3-F43FFFC7216B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="630" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>URL</t>
   </si>
@@ -78,18 +78,6 @@
   </si>
   <si>
     <t>COP</t>
-  </si>
-  <si>
-    <t>CNY</t>
-  </si>
-  <si>
-    <t>JPY</t>
-  </si>
-  <si>
-    <t>BRL</t>
-  </si>
-  <si>
-    <t>KRW</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -198,7 +186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -210,7 +198,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -282,7 +269,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}" name="Tabla1" displayName="Tabla1" ref="A1:C9" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}" name="Tabla1" displayName="Tabla1" ref="A1:C3" totalsRowShown="0" headerRowDxfId="4">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8451EFC4-375F-4EF1-B2A2-7878C751B650}" name="URL" dataDxfId="3">
       <calculatedColumnFormula>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</calculatedColumnFormula>
@@ -630,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -715,16 +702,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="str">
-        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
-        <v>https://www.oanda.com/currency-converter/es/?from=CNY&amp;to=USD&amp;amount=1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A4" s="1"/>
       <c r="F4" t="s">
         <v>9</v>
       </c>
@@ -739,131 +717,86 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="str">
-        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
-        <v>https://www.oanda.com/currency-converter/es/?from=JPY&amp;to=USD&amp;amount=1</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="1"/>
+      <c r="F5" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="str">
-        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
-        <v>https://www.oanda.com/currency-converter/es/?from=CNY&amp;to=COP&amp;amount=1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="str">
-        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
-        <v>https://www.oanda.com/currency-converter/es/?from=JPY&amp;to=COP&amp;amount=1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="str">
-        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
-        <v>https://www.oanda.com/currency-converter/es/?from=BRL&amp;to=USD&amp;amount=1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
+      <c r="A8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="str">
-        <f>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</f>
-        <v>https://www.oanda.com/currency-converter/es/?from=KRW&amp;to=USD&amp;amount=1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
+      <c r="A9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s">
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="D10" s="1"/>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G10" t="s">
         <v>4</v>
@@ -872,28 +805,27 @@
         <v>14</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F16" s="1"/>

</xml_diff>

<commit_message>
Correcion de valores con punto y coma
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Tasas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24759BC0-141E-4DC3-8FE9-CF0894296954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDD1F5E-C9A0-47EE-8433-C20D06B3CCD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t>URL</t>
   </si>
@@ -68,15 +68,6 @@
     <t>CLP</t>
   </si>
   <si>
-    <t>#\32 225 &gt; div &gt; div &gt; span:nth-child(2)</t>
-  </si>
-  <si>
-    <t>#lblValor1_3</t>
-  </si>
-  <si>
-    <t>#lblValor1_5</t>
-  </si>
-  <si>
     <t>COP</t>
   </si>
   <si>
@@ -89,9 +80,6 @@
     <t>CLP (Oanda)</t>
   </si>
   <si>
-    <t>#cc-time-series-plot &gt; div &gt; div &gt; div:nth-child(2) &gt; div &gt; table &gt; tbody &gt; tr:nth-child(2) &gt; td:nth-child(3)</t>
-  </si>
-  <si>
     <t>https://www.oanda.com/currency-converter/es/?from=EUR&amp;to=CLP&amp;amount=1</t>
   </si>
   <si>
@@ -101,27 +89,15 @@
     <t>CRC</t>
   </si>
   <si>
-    <t>#theTable400 &gt; tbody &gt; tr:nth-child(2) &gt; td:nth-child(3) &gt; table &gt; tbody &gt; tr &gt; td &gt; table &gt; tbody &gt; tr:nth-child(30) &gt; td</t>
-  </si>
-  <si>
     <t>https://www.sbs.gob.pe/app/pp/sistip_portal/paginas/publicacion/tipocambiopromedio.aspx</t>
   </si>
   <si>
     <t>PEN</t>
   </si>
   <si>
-    <t>#ctl00_cphContent_rgTipoCambio_ctl00__0 &gt; td:nth-child(3)</t>
-  </si>
-  <si>
-    <t>#ctl00_cphContent_rgTipoCambio_ctl00__6 &gt; td:nth-child(3)</t>
-  </si>
-  <si>
     <t>https://www.banrep.gov.co/es</t>
   </si>
   <si>
-    <t>#block-banrepindicatorsblock &gt; div &gt; div.column.large-3.indicator.indicator--trm &gt; div.indicator__value &gt; a</t>
-  </si>
-  <si>
     <t>#ctl00_ctl63_g_8899d5e6_dcfc_4225_83da_4a766737a409 &gt; div &gt; div &gt; div</t>
   </si>
   <si>
@@ -180,13 +156,40 @@
   </si>
   <si>
     <t>CO75</t>
+  </si>
+  <si>
+    <t>//*[@id='lblValor1_5']</t>
+  </si>
+  <si>
+    <t>//*[@id="ctl00_ctl63_g_0723770d_f942_45cc_80db_28dc7fa543a2_ctl00_lstCotizaciones"]/tbody/tr[1]/td[3]</t>
+  </si>
+  <si>
+    <t>//*[@id='lblValor1_3']</t>
+  </si>
+  <si>
+    <t>//*[@id="cc-time-series-plot"]/div/div/div[2]/div/table/tbody/tr[2]/td[3]</t>
+  </si>
+  <si>
+    <t>//*[@id="theTable400"]/tbody/tr[2]/td[3]/table/tbody/tr/td/table/tbody/tr[30]/td</t>
+  </si>
+  <si>
+    <t>//*[@id="ctl00_cphContent_rgTipoCambio_ctl00__0"]/td[3]</t>
+  </si>
+  <si>
+    <t>//*[@id="ctl00_cphContent_rgTipoCambio_ctl00__6"]/td[3]</t>
+  </si>
+  <si>
+    <t>https://www.bcu.gub.uy/Estadisticas-e-Indicadores/Paginas/Cotizaciones.aspx</t>
+  </si>
+  <si>
+    <t>//*[@id="block-banrepindicatorsblock"]/div/div[2]/div[2]/a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,6 +234,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -269,18 +279,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -347,25 +372,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}" name="Tabla1" displayName="Tabla1" ref="A1:C3" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8A05848-56F6-4709-8EDE-0EA08E8EB152}" name="Tabla1" displayName="Tabla1" ref="A1:C3" totalsRowShown="0" headerRowDxfId="6">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8451EFC4-375F-4EF1-B2A2-7878C751B650}" name="URL" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{8451EFC4-375F-4EF1-B2A2-7878C751B650}" name="URL" dataDxfId="5">
       <calculatedColumnFormula>+CONCATENATE("https://www.oanda.com/currency-converter/es/?from=",Tabla1[[#This Row],[TO]],"&amp;to=",Tabla1[[#This Row],[FROM]],"&amp;amount=1")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{30A2418A-0C4F-4155-8F56-B5A5880AB528}" name="TO" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{1A1624D6-F818-4D44-A135-7EBB14A8DD57}" name="FROM" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{30A2418A-0C4F-4155-8F56-B5A5880AB528}" name="TO" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{1A1624D6-F818-4D44-A135-7EBB14A8DD57}" name="FROM" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0C0D46E7-F487-476A-BDD3-0C37CA786D97}" name="Tabla2" displayName="Tabla2" ref="F1:I10" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0C0D46E7-F487-476A-BDD3-0C37CA786D97}" name="Tabla2" displayName="Tabla2" ref="F1:I10" totalsRowShown="0" headerRowDxfId="2">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{ABE21EB8-1A09-47F7-8813-64338A7A4AE6}" name="URL Bank"/>
     <tableColumn id="2" xr3:uid="{37FCEC7A-FCE2-448E-896B-F917DDB7E005}" name="TO"/>
     <tableColumn id="3" xr3:uid="{013531B8-09B0-422B-A9E9-5DA7DACA8D07}" name="FROM"/>
-    <tableColumn id="4" xr3:uid="{3459D215-8DCE-4383-A927-75D242284818}" name="HTML"/>
+    <tableColumn id="4" xr3:uid="{3459D215-8DCE-4383-A927-75D242284818}" name="HTML" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -716,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -746,7 +771,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>5</v>
@@ -762,13 +787,13 @@
       </c>
       <c r="J1" s="4"/>
       <c r="K1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="M1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -783,11 +808,11 @@
         <v>4</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
+      <c r="E2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -795,17 +820,17 @@
       <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>11</v>
+      <c r="I2" t="s">
+        <v>42</v>
       </c>
       <c r="K2" t="s">
         <v>7</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="M2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -817,10 +842,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>45</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>9</v>
@@ -831,23 +856,23 @@
       <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>12</v>
+      <c r="I3" t="s">
+        <v>43</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="M3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="E4" s="7" t="s">
-        <v>45</v>
+      <c r="E4" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -858,151 +883,152 @@
       <c r="H4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>13</v>
+      <c r="I4" t="s">
+        <v>41</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="M4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="E5" s="7" t="s">
-        <v>45</v>
+      <c r="E5" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="M5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="E6" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>19</v>
+      <c r="E6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="M6" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="E7" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>20</v>
+      <c r="E7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s">
-        <v>22</v>
+        <v>14</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="E8" s="7" t="s">
-        <v>44</v>
+      <c r="E8" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="E9" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>23</v>
+      <c r="E9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" t="s">
-        <v>27</v>
+      <c r="E10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="G10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1013,7 +1039,7 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I13" s="1"/>
       <c r="L13" s="1"/>
@@ -1030,6 +1056,7 @@
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F16" s="1"/>
       <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="6:12" x14ac:dyDescent="0.25">
       <c r="K17" s="1"/>
@@ -1052,12 +1079,12 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1" xr:uid="{9035CC73-D16E-486C-A6CB-0843C216291F}"/>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{9035CC73-D16E-486C-A6CB-0843C216291F}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{C147C48E-B3E2-42FE-B4A5-2D1233F619AA}"/>
     <hyperlink ref="K4" r:id="rId3" xr:uid="{26EA0ED3-5737-4185-B57C-870F96C196EC}"/>
     <hyperlink ref="K5" r:id="rId4" xr:uid="{45B40474-14F1-4FB7-8CD6-6F5C8A7EE7EE}"/>
     <hyperlink ref="K6" r:id="rId5" xr:uid="{766F0DD0-AEDE-49DF-9D92-DD0B8352F7BB}"/>
-    <hyperlink ref="F9" r:id="rId6" xr:uid="{AA6BBAEF-AA80-4E1A-AC8B-43C8E19D9DDB}"/>
+    <hyperlink ref="F10" r:id="rId6" xr:uid="{AA6BBAEF-AA80-4E1A-AC8B-43C8E19D9DDB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>